<commit_message>
Removed "start" and "end"  legend from 20by20 maze
</commit_message>
<xml_diff>
--- a/maze.xlsx
+++ b/maze.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science\Search Algorithms\depth_first_search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science\Search Algorithms\maze_path_search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03010667-FFE5-4F90-A7A4-94A3BB8F0533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8432397E-7613-4D23-A4B0-C21426F9DF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="123">
   <si>
     <t>A</t>
   </si>
@@ -117,12 +117,6 @@
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t>FN</t>
   </si>
   <si>
     <t>#</t>
@@ -582,7 +576,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,12 +754,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -957,15 +945,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1022,19 +1009,19 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1351,7 +1338,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1361,78 +1348,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" cm="1">
+      <c r="A2" s="3" cm="1">
         <f t="array" ref="A2:A21">_xlfn.SEQUENCE(20)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1444,15 +1429,15 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -1460,73 +1445,73 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1534,83 +1519,83 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1623,166 +1608,166 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
@@ -1790,152 +1775,152 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1943,30 +1928,30 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="1"/>
@@ -1976,293 +1961,293 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U15" s="1"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U17" s="1"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1"/>
@@ -2276,10 +2261,10 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -2291,66 +2276,64 @@
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="U21" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:U21">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"#"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2376,316 +2359,316 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7" cm="1">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" cm="1">
         <f t="array" ref="B1:CX1">_xlfn.SEQUENCE(1,101)</f>
         <v>1</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="6">
         <v>2</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="7">
+      <c r="E1" s="6">
         <v>4</v>
       </c>
-      <c r="F1" s="7">
+      <c r="F1" s="6">
         <v>5</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1" s="6">
         <v>6</v>
       </c>
-      <c r="H1" s="7">
+      <c r="H1" s="6">
         <v>7</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="6">
         <v>8</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J1" s="6">
         <v>9</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K1" s="6">
         <v>10</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="6">
         <v>11</v>
       </c>
-      <c r="M1" s="7">
+      <c r="M1" s="6">
         <v>12</v>
       </c>
-      <c r="N1" s="7">
+      <c r="N1" s="6">
         <v>13</v>
       </c>
-      <c r="O1" s="7">
+      <c r="O1" s="6">
         <v>14</v>
       </c>
-      <c r="P1" s="7">
+      <c r="P1" s="6">
         <v>15</v>
       </c>
-      <c r="Q1" s="7">
+      <c r="Q1" s="6">
         <v>16</v>
       </c>
-      <c r="R1" s="7">
+      <c r="R1" s="6">
         <v>17</v>
       </c>
-      <c r="S1" s="7">
+      <c r="S1" s="6">
         <v>18</v>
       </c>
-      <c r="T1" s="7">
+      <c r="T1" s="6">
         <v>19</v>
       </c>
-      <c r="U1" s="7">
+      <c r="U1" s="6">
         <v>20</v>
       </c>
-      <c r="V1" s="7">
+      <c r="V1" s="6">
         <v>21</v>
       </c>
-      <c r="W1" s="7">
+      <c r="W1" s="6">
         <v>22</v>
       </c>
-      <c r="X1" s="7">
+      <c r="X1" s="6">
         <v>23</v>
       </c>
-      <c r="Y1" s="7">
+      <c r="Y1" s="6">
         <v>24</v>
       </c>
-      <c r="Z1" s="7">
+      <c r="Z1" s="6">
         <v>25</v>
       </c>
-      <c r="AA1" s="7">
+      <c r="AA1" s="6">
         <v>26</v>
       </c>
-      <c r="AB1" s="7">
+      <c r="AB1" s="6">
         <v>27</v>
       </c>
-      <c r="AC1" s="7">
+      <c r="AC1" s="6">
         <v>28</v>
       </c>
-      <c r="AD1" s="7">
+      <c r="AD1" s="6">
         <v>29</v>
       </c>
-      <c r="AE1" s="7">
+      <c r="AE1" s="6">
         <v>30</v>
       </c>
-      <c r="AF1" s="7">
+      <c r="AF1" s="6">
         <v>31</v>
       </c>
-      <c r="AG1" s="7">
+      <c r="AG1" s="6">
         <v>32</v>
       </c>
-      <c r="AH1" s="7">
+      <c r="AH1" s="6">
         <v>33</v>
       </c>
-      <c r="AI1" s="7">
+      <c r="AI1" s="6">
         <v>34</v>
       </c>
-      <c r="AJ1" s="7">
+      <c r="AJ1" s="6">
         <v>35</v>
       </c>
-      <c r="AK1" s="7">
+      <c r="AK1" s="6">
         <v>36</v>
       </c>
-      <c r="AL1" s="7">
+      <c r="AL1" s="6">
         <v>37</v>
       </c>
-      <c r="AM1" s="7">
+      <c r="AM1" s="6">
         <v>38</v>
       </c>
-      <c r="AN1" s="7">
+      <c r="AN1" s="6">
         <v>39</v>
       </c>
-      <c r="AO1" s="7">
+      <c r="AO1" s="6">
         <v>40</v>
       </c>
-      <c r="AP1" s="7">
+      <c r="AP1" s="6">
         <v>41</v>
       </c>
-      <c r="AQ1" s="7">
+      <c r="AQ1" s="6">
         <v>42</v>
       </c>
-      <c r="AR1" s="7">
+      <c r="AR1" s="6">
         <v>43</v>
       </c>
-      <c r="AS1" s="7">
+      <c r="AS1" s="6">
         <v>44</v>
       </c>
-      <c r="AT1" s="7">
+      <c r="AT1" s="6">
         <v>45</v>
       </c>
-      <c r="AU1" s="7">
+      <c r="AU1" s="6">
         <v>46</v>
       </c>
-      <c r="AV1" s="7">
+      <c r="AV1" s="6">
         <v>47</v>
       </c>
-      <c r="AW1" s="7">
+      <c r="AW1" s="6">
         <v>48</v>
       </c>
-      <c r="AX1" s="7">
+      <c r="AX1" s="6">
         <v>49</v>
       </c>
-      <c r="AY1" s="7">
+      <c r="AY1" s="6">
         <v>50</v>
       </c>
-      <c r="AZ1" s="6">
+      <c r="AZ1" s="5">
         <v>51</v>
       </c>
-      <c r="BA1" s="6">
+      <c r="BA1" s="5">
         <v>52</v>
       </c>
-      <c r="BB1" s="6">
+      <c r="BB1" s="5">
         <v>53</v>
       </c>
-      <c r="BC1" s="6">
+      <c r="BC1" s="5">
         <v>54</v>
       </c>
-      <c r="BD1" s="6">
+      <c r="BD1" s="5">
         <v>55</v>
       </c>
-      <c r="BE1" s="6">
+      <c r="BE1" s="5">
         <v>56</v>
       </c>
-      <c r="BF1" s="6">
+      <c r="BF1" s="5">
         <v>57</v>
       </c>
-      <c r="BG1" s="6">
+      <c r="BG1" s="5">
         <v>58</v>
       </c>
-      <c r="BH1" s="6">
+      <c r="BH1" s="5">
         <v>59</v>
       </c>
-      <c r="BI1" s="6">
+      <c r="BI1" s="5">
         <v>60</v>
       </c>
-      <c r="BJ1" s="6">
+      <c r="BJ1" s="5">
         <v>61</v>
       </c>
-      <c r="BK1" s="6">
+      <c r="BK1" s="5">
         <v>62</v>
       </c>
-      <c r="BL1" s="6">
+      <c r="BL1" s="5">
         <v>63</v>
       </c>
-      <c r="BM1" s="6">
+      <c r="BM1" s="5">
         <v>64</v>
       </c>
-      <c r="BN1" s="6">
+      <c r="BN1" s="5">
         <v>65</v>
       </c>
-      <c r="BO1" s="6">
+      <c r="BO1" s="5">
         <v>66</v>
       </c>
-      <c r="BP1" s="6">
+      <c r="BP1" s="5">
         <v>67</v>
       </c>
-      <c r="BQ1" s="6">
+      <c r="BQ1" s="5">
         <v>68</v>
       </c>
-      <c r="BR1" s="6">
+      <c r="BR1" s="5">
         <v>69</v>
       </c>
-      <c r="BS1" s="6">
+      <c r="BS1" s="5">
         <v>70</v>
       </c>
-      <c r="BT1" s="6">
+      <c r="BT1" s="5">
         <v>71</v>
       </c>
-      <c r="BU1" s="6">
+      <c r="BU1" s="5">
         <v>72</v>
       </c>
-      <c r="BV1" s="6">
+      <c r="BV1" s="5">
         <v>73</v>
       </c>
-      <c r="BW1" s="6">
+      <c r="BW1" s="5">
         <v>74</v>
       </c>
-      <c r="BX1" s="6">
+      <c r="BX1" s="5">
         <v>75</v>
       </c>
-      <c r="BY1" s="6">
+      <c r="BY1" s="5">
         <v>76</v>
       </c>
-      <c r="BZ1" s="6">
+      <c r="BZ1" s="5">
         <v>77</v>
       </c>
-      <c r="CA1" s="6">
+      <c r="CA1" s="5">
         <v>78</v>
       </c>
-      <c r="CB1" s="6">
+      <c r="CB1" s="5">
         <v>79</v>
       </c>
-      <c r="CC1" s="6">
+      <c r="CC1" s="5">
         <v>80</v>
       </c>
-      <c r="CD1" s="6">
+      <c r="CD1" s="5">
         <v>81</v>
       </c>
-      <c r="CE1" s="6">
+      <c r="CE1" s="5">
         <v>82</v>
       </c>
-      <c r="CF1" s="6">
+      <c r="CF1" s="5">
         <v>83</v>
       </c>
-      <c r="CG1" s="6">
+      <c r="CG1" s="5">
         <v>84</v>
       </c>
-      <c r="CH1" s="6">
+      <c r="CH1" s="5">
         <v>85</v>
       </c>
-      <c r="CI1" s="6">
+      <c r="CI1" s="5">
         <v>86</v>
       </c>
-      <c r="CJ1" s="6">
+      <c r="CJ1" s="5">
         <v>87</v>
       </c>
-      <c r="CK1" s="6">
+      <c r="CK1" s="5">
         <v>88</v>
       </c>
-      <c r="CL1" s="6">
+      <c r="CL1" s="5">
         <v>89</v>
       </c>
-      <c r="CM1" s="6">
+      <c r="CM1" s="5">
         <v>90</v>
       </c>
-      <c r="CN1" s="6">
+      <c r="CN1" s="5">
         <v>91</v>
       </c>
-      <c r="CO1" s="6">
+      <c r="CO1" s="5">
         <v>92</v>
       </c>
-      <c r="CP1" s="6">
+      <c r="CP1" s="5">
         <v>93</v>
       </c>
-      <c r="CQ1" s="6">
+      <c r="CQ1" s="5">
         <v>94</v>
       </c>
-      <c r="CR1" s="6">
+      <c r="CR1" s="5">
         <v>95</v>
       </c>
-      <c r="CS1" s="6">
+      <c r="CS1" s="5">
         <v>96</v>
       </c>
-      <c r="CT1" s="6">
+      <c r="CT1" s="5">
         <v>97</v>
       </c>
-      <c r="CU1" s="6">
+      <c r="CU1" s="5">
         <v>98</v>
       </c>
-      <c r="CV1" s="6">
+      <c r="CV1" s="5">
         <v>99</v>
       </c>
-      <c r="CW1" s="6">
+      <c r="CW1" s="5">
         <v>100</v>
       </c>
-      <c r="CX1" s="6">
+      <c r="CX1" s="5">
         <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" cm="1">
+      <c r="A2" s="5" cm="1">
         <f t="array" ref="A2:A102">_xlfn.SEQUENCE(101)</f>
         <v>1</v>
       </c>
@@ -2995,7 +2978,7 @@
       </c>
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" t="str" cm="1">
@@ -3304,7 +3287,7 @@
       </c>
     </row>
     <row r="4" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" t="str" cm="1">
@@ -3613,7 +3596,7 @@
       </c>
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" t="str" cm="1">
@@ -3922,7 +3905,7 @@
       </c>
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" t="str" cm="1">
@@ -4231,7 +4214,7 @@
       </c>
     </row>
     <row r="7" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" t="str" cm="1">
@@ -4540,7 +4523,7 @@
       </c>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" t="str" cm="1">
@@ -4849,7 +4832,7 @@
       </c>
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" t="str" cm="1">
@@ -5158,7 +5141,7 @@
       </c>
     </row>
     <row r="10" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" t="str" cm="1">
@@ -5467,7 +5450,7 @@
       </c>
     </row>
     <row r="11" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" t="str" cm="1">
@@ -5776,7 +5759,7 @@
       </c>
     </row>
     <row r="12" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" t="str" cm="1">
@@ -6085,7 +6068,7 @@
       </c>
     </row>
     <row r="13" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" t="str" cm="1">
@@ -6394,7 +6377,7 @@
       </c>
     </row>
     <row r="14" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" t="str" cm="1">
@@ -6703,7 +6686,7 @@
       </c>
     </row>
     <row r="15" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" t="str" cm="1">
@@ -7012,7 +6995,7 @@
       </c>
     </row>
     <row r="16" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" t="str" cm="1">
@@ -7321,7 +7304,7 @@
       </c>
     </row>
     <row r="17" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" t="str" cm="1">
@@ -7630,7 +7613,7 @@
       </c>
     </row>
     <row r="18" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" t="str" cm="1">
@@ -7939,7 +7922,7 @@
       </c>
     </row>
     <row r="19" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" t="str" cm="1">
@@ -8248,7 +8231,7 @@
       </c>
     </row>
     <row r="20" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" t="str" cm="1">
@@ -8557,7 +8540,7 @@
       </c>
     </row>
     <row r="21" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" t="str" cm="1">
@@ -8866,7 +8849,7 @@
       </c>
     </row>
     <row r="22" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" t="str" cm="1">
@@ -9175,7 +9158,7 @@
       </c>
     </row>
     <row r="23" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" t="str" cm="1">
@@ -9484,7 +9467,7 @@
       </c>
     </row>
     <row r="24" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" t="str" cm="1">
@@ -9793,7 +9776,7 @@
       </c>
     </row>
     <row r="25" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" t="str" cm="1">
@@ -10102,7 +10085,7 @@
       </c>
     </row>
     <row r="26" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" t="str" cm="1">
@@ -10411,7 +10394,7 @@
       </c>
     </row>
     <row r="27" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" t="str" cm="1">
@@ -10720,7 +10703,7 @@
       </c>
     </row>
     <row r="28" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" t="str" cm="1">
@@ -11029,7 +11012,7 @@
       </c>
     </row>
     <row r="29" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" t="str" cm="1">
@@ -11338,7 +11321,7 @@
       </c>
     </row>
     <row r="30" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30" t="str" cm="1">
@@ -11647,7 +11630,7 @@
       </c>
     </row>
     <row r="31" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" t="str" cm="1">
@@ -11956,7 +11939,7 @@
       </c>
     </row>
     <row r="32" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32" t="str" cm="1">
@@ -12265,7 +12248,7 @@
       </c>
     </row>
     <row r="33" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33" t="str" cm="1">
@@ -12574,7 +12557,7 @@
       </c>
     </row>
     <row r="34" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34" t="str" cm="1">
@@ -12883,7 +12866,7 @@
       </c>
     </row>
     <row r="35" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35" t="str" cm="1">
@@ -13192,7 +13175,7 @@
       </c>
     </row>
     <row r="36" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="B36" t="str" cm="1">
@@ -13501,7 +13484,7 @@
       </c>
     </row>
     <row r="37" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37" t="str" cm="1">
@@ -13810,7 +13793,7 @@
       </c>
     </row>
     <row r="38" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38" t="str" cm="1">
@@ -14119,7 +14102,7 @@
       </c>
     </row>
     <row r="39" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A39" s="6">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39" t="str" cm="1">
@@ -14428,7 +14411,7 @@
       </c>
     </row>
     <row r="40" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A40" s="6">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40" t="str" cm="1">
@@ -14737,7 +14720,7 @@
       </c>
     </row>
     <row r="41" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41" t="str" cm="1">
@@ -15046,7 +15029,7 @@
       </c>
     </row>
     <row r="42" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
+      <c r="A42" s="5">
         <v>41</v>
       </c>
       <c r="B42" t="str" cm="1">
@@ -15355,7 +15338,7 @@
       </c>
     </row>
     <row r="43" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A43" s="6">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" t="str" cm="1">
@@ -15664,7 +15647,7 @@
       </c>
     </row>
     <row r="44" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
       <c r="B44" t="str" cm="1">
@@ -15973,7 +15956,7 @@
       </c>
     </row>
     <row r="45" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45" t="str" cm="1">
@@ -16282,7 +16265,7 @@
       </c>
     </row>
     <row r="46" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A46" s="6">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
       <c r="B46" t="str" cm="1">
@@ -16591,7 +16574,7 @@
       </c>
     </row>
     <row r="47" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A47" s="6">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
       <c r="B47" t="str" cm="1">
@@ -16900,7 +16883,7 @@
       </c>
     </row>
     <row r="48" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A48" s="6">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
       <c r="B48" t="str" cm="1">
@@ -17209,7 +17192,7 @@
       </c>
     </row>
     <row r="49" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A49" s="6">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
       <c r="B49" t="str" cm="1">
@@ -17518,7 +17501,7 @@
       </c>
     </row>
     <row r="50" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A50" s="6">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="B50" t="str" cm="1">
@@ -17827,7 +17810,7 @@
       </c>
     </row>
     <row r="51" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A51" s="6">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
       <c r="B51" t="str" cm="1">
@@ -18136,7 +18119,7 @@
       </c>
     </row>
     <row r="52" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A52" s="6">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
       <c r="B52" t="str" cm="1">
@@ -18445,7 +18428,7 @@
       </c>
     </row>
     <row r="53" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A53" s="6">
+      <c r="A53" s="5">
         <v>52</v>
       </c>
       <c r="B53" t="str" cm="1">
@@ -18754,7 +18737,7 @@
       </c>
     </row>
     <row r="54" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A54" s="6">
+      <c r="A54" s="5">
         <v>53</v>
       </c>
       <c r="B54" t="str" cm="1">
@@ -19063,7 +19046,7 @@
       </c>
     </row>
     <row r="55" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A55" s="6">
+      <c r="A55" s="5">
         <v>54</v>
       </c>
       <c r="B55" t="str" cm="1">
@@ -19372,7 +19355,7 @@
       </c>
     </row>
     <row r="56" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A56" s="6">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
       <c r="B56" t="str" cm="1">
@@ -19681,7 +19664,7 @@
       </c>
     </row>
     <row r="57" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A57" s="6">
+      <c r="A57" s="5">
         <v>56</v>
       </c>
       <c r="B57" t="str" cm="1">
@@ -19990,7 +19973,7 @@
       </c>
     </row>
     <row r="58" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A58" s="6">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
       <c r="B58" t="str" cm="1">
@@ -20299,7 +20282,7 @@
       </c>
     </row>
     <row r="59" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A59" s="6">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
       <c r="B59" t="str" cm="1">
@@ -20608,7 +20591,7 @@
       </c>
     </row>
     <row r="60" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A60" s="6">
+      <c r="A60" s="5">
         <v>59</v>
       </c>
       <c r="B60" t="str" cm="1">
@@ -20917,7 +20900,7 @@
       </c>
     </row>
     <row r="61" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A61" s="6">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
       <c r="B61" t="str" cm="1">
@@ -21226,7 +21209,7 @@
       </c>
     </row>
     <row r="62" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A62" s="6">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
       <c r="B62" t="str" cm="1">
@@ -21535,7 +21518,7 @@
       </c>
     </row>
     <row r="63" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A63" s="6">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
       <c r="B63" t="str" cm="1">
@@ -21844,7 +21827,7 @@
       </c>
     </row>
     <row r="64" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A64" s="6">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
       <c r="B64" t="str" cm="1">
@@ -22153,7 +22136,7 @@
       </c>
     </row>
     <row r="65" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A65" s="6">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
       <c r="B65" t="str" cm="1">
@@ -22462,7 +22445,7 @@
       </c>
     </row>
     <row r="66" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A66" s="6">
+      <c r="A66" s="5">
         <v>65</v>
       </c>
       <c r="B66" t="str" cm="1">
@@ -22771,7 +22754,7 @@
       </c>
     </row>
     <row r="67" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A67" s="6">
+      <c r="A67" s="5">
         <v>66</v>
       </c>
       <c r="B67" t="str" cm="1">
@@ -23080,7 +23063,7 @@
       </c>
     </row>
     <row r="68" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A68" s="6">
+      <c r="A68" s="5">
         <v>67</v>
       </c>
       <c r="B68" t="str" cm="1">
@@ -23389,7 +23372,7 @@
       </c>
     </row>
     <row r="69" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A69" s="6">
+      <c r="A69" s="5">
         <v>68</v>
       </c>
       <c r="B69" t="str" cm="1">
@@ -23698,7 +23681,7 @@
       </c>
     </row>
     <row r="70" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A70" s="6">
+      <c r="A70" s="5">
         <v>69</v>
       </c>
       <c r="B70" t="str" cm="1">
@@ -24007,7 +23990,7 @@
       </c>
     </row>
     <row r="71" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A71" s="6">
+      <c r="A71" s="5">
         <v>70</v>
       </c>
       <c r="B71" t="str" cm="1">
@@ -24316,7 +24299,7 @@
       </c>
     </row>
     <row r="72" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A72" s="6">
+      <c r="A72" s="5">
         <v>71</v>
       </c>
       <c r="B72" t="str" cm="1">
@@ -24625,7 +24608,7 @@
       </c>
     </row>
     <row r="73" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A73" s="6">
+      <c r="A73" s="5">
         <v>72</v>
       </c>
       <c r="B73" t="str" cm="1">
@@ -24934,7 +24917,7 @@
       </c>
     </row>
     <row r="74" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A74" s="6">
+      <c r="A74" s="5">
         <v>73</v>
       </c>
       <c r="B74" t="str" cm="1">
@@ -25243,7 +25226,7 @@
       </c>
     </row>
     <row r="75" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A75" s="6">
+      <c r="A75" s="5">
         <v>74</v>
       </c>
       <c r="B75" t="str" cm="1">
@@ -25552,7 +25535,7 @@
       </c>
     </row>
     <row r="76" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A76" s="6">
+      <c r="A76" s="5">
         <v>75</v>
       </c>
       <c r="B76" t="str" cm="1">
@@ -25861,7 +25844,7 @@
       </c>
     </row>
     <row r="77" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A77" s="6">
+      <c r="A77" s="5">
         <v>76</v>
       </c>
       <c r="B77" t="str" cm="1">
@@ -26170,7 +26153,7 @@
       </c>
     </row>
     <row r="78" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A78" s="6">
+      <c r="A78" s="5">
         <v>77</v>
       </c>
       <c r="B78" t="str" cm="1">
@@ -26479,7 +26462,7 @@
       </c>
     </row>
     <row r="79" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A79" s="6">
+      <c r="A79" s="5">
         <v>78</v>
       </c>
       <c r="B79" t="str" cm="1">
@@ -26788,7 +26771,7 @@
       </c>
     </row>
     <row r="80" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A80" s="6">
+      <c r="A80" s="5">
         <v>79</v>
       </c>
       <c r="B80" t="str" cm="1">
@@ -27097,7 +27080,7 @@
       </c>
     </row>
     <row r="81" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A81" s="6">
+      <c r="A81" s="5">
         <v>80</v>
       </c>
       <c r="B81" t="str" cm="1">
@@ -27406,7 +27389,7 @@
       </c>
     </row>
     <row r="82" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A82" s="6">
+      <c r="A82" s="5">
         <v>81</v>
       </c>
       <c r="B82" t="str" cm="1">
@@ -27715,7 +27698,7 @@
       </c>
     </row>
     <row r="83" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A83" s="6">
+      <c r="A83" s="5">
         <v>82</v>
       </c>
       <c r="B83" t="str" cm="1">
@@ -28024,7 +28007,7 @@
       </c>
     </row>
     <row r="84" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A84" s="6">
+      <c r="A84" s="5">
         <v>83</v>
       </c>
       <c r="B84" t="str" cm="1">
@@ -28333,7 +28316,7 @@
       </c>
     </row>
     <row r="85" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A85" s="6">
+      <c r="A85" s="5">
         <v>84</v>
       </c>
       <c r="B85" t="str" cm="1">
@@ -28642,7 +28625,7 @@
       </c>
     </row>
     <row r="86" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A86" s="6">
+      <c r="A86" s="5">
         <v>85</v>
       </c>
       <c r="B86" t="str" cm="1">
@@ -28951,7 +28934,7 @@
       </c>
     </row>
     <row r="87" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A87" s="6">
+      <c r="A87" s="5">
         <v>86</v>
       </c>
       <c r="B87" t="str" cm="1">
@@ -29260,7 +29243,7 @@
       </c>
     </row>
     <row r="88" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A88" s="6">
+      <c r="A88" s="5">
         <v>87</v>
       </c>
       <c r="B88" t="str" cm="1">
@@ -29569,7 +29552,7 @@
       </c>
     </row>
     <row r="89" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A89" s="6">
+      <c r="A89" s="5">
         <v>88</v>
       </c>
       <c r="B89" t="str" cm="1">
@@ -29878,7 +29861,7 @@
       </c>
     </row>
     <row r="90" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A90" s="6">
+      <c r="A90" s="5">
         <v>89</v>
       </c>
       <c r="B90" t="str" cm="1">
@@ -30187,7 +30170,7 @@
       </c>
     </row>
     <row r="91" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A91" s="6">
+      <c r="A91" s="5">
         <v>90</v>
       </c>
       <c r="B91" t="str" cm="1">
@@ -30496,7 +30479,7 @@
       </c>
     </row>
     <row r="92" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A92" s="6">
+      <c r="A92" s="5">
         <v>91</v>
       </c>
       <c r="B92" t="str" cm="1">
@@ -30805,7 +30788,7 @@
       </c>
     </row>
     <row r="93" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A93" s="6">
+      <c r="A93" s="5">
         <v>92</v>
       </c>
       <c r="B93" t="str" cm="1">
@@ -31114,7 +31097,7 @@
       </c>
     </row>
     <row r="94" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A94" s="6">
+      <c r="A94" s="5">
         <v>93</v>
       </c>
       <c r="B94" t="str" cm="1">
@@ -31423,7 +31406,7 @@
       </c>
     </row>
     <row r="95" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A95" s="6">
+      <c r="A95" s="5">
         <v>94</v>
       </c>
       <c r="B95" t="str" cm="1">
@@ -31732,7 +31715,7 @@
       </c>
     </row>
     <row r="96" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A96" s="6">
+      <c r="A96" s="5">
         <v>95</v>
       </c>
       <c r="B96" t="str" cm="1">
@@ -32041,7 +32024,7 @@
       </c>
     </row>
     <row r="97" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A97" s="6">
+      <c r="A97" s="5">
         <v>96</v>
       </c>
       <c r="B97" t="str" cm="1">
@@ -32350,7 +32333,7 @@
       </c>
     </row>
     <row r="98" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A98" s="6">
+      <c r="A98" s="5">
         <v>97</v>
       </c>
       <c r="B98" t="str" cm="1">
@@ -32659,7 +32642,7 @@
       </c>
     </row>
     <row r="99" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A99" s="6">
+      <c r="A99" s="5">
         <v>98</v>
       </c>
       <c r="B99" t="str" cm="1">
@@ -32968,7 +32951,7 @@
       </c>
     </row>
     <row r="100" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A100" s="6">
+      <c r="A100" s="5">
         <v>99</v>
       </c>
       <c r="B100" t="str" cm="1">
@@ -33277,7 +33260,7 @@
       </c>
     </row>
     <row r="101" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A101" s="6">
+      <c r="A101" s="5">
         <v>100</v>
       </c>
       <c r="B101" t="str" cm="1">
@@ -33586,7 +33569,7 @@
       </c>
     </row>
     <row r="102" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A102" s="6">
+      <c r="A102" s="5">
         <v>101</v>
       </c>
       <c r="B102" t="str" cm="1">
@@ -33896,7 +33879,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:CX102">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33919,7 +33902,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="str">
+      <c r="A1" s="7" t="str">
         <f>HYPERLINK("https://www.dcode.fr/maze-generator","SOURCE")</f>
         <v>SOURCE</v>
       </c>
@@ -34230,7 +34213,7 @@
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" ref="B2:CX2">MID(A2,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -34539,7 +34522,7 @@
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="str" cm="1">
         <f t="array" ref="B3:CX3">MID(A3,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -34848,7 +34831,7 @@
     </row>
     <row r="4" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="str" cm="1">
         <f t="array" ref="B4:CX4">MID(A4,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -35157,7 +35140,7 @@
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="str" cm="1">
         <f t="array" ref="B5:CX5">MID(A5,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -35466,7 +35449,7 @@
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="str" cm="1">
         <f t="array" ref="B6:CX6">MID(A6,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -35775,7 +35758,7 @@
     </row>
     <row r="7" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" t="str" cm="1">
         <f t="array" ref="B7:CX7">MID(A7,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -36084,7 +36067,7 @@
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="str" cm="1">
         <f t="array" ref="B8:CX8">MID(A8,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -36393,7 +36376,7 @@
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" t="str" cm="1">
         <f t="array" ref="B9:CX9">MID(A9,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -36702,7 +36685,7 @@
     </row>
     <row r="10" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:CX10">MID(A10,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -37011,7 +36994,7 @@
     </row>
     <row r="11" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="str" cm="1">
         <f t="array" ref="B11:CX11">MID(A11,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -37320,7 +37303,7 @@
     </row>
     <row r="12" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="str" cm="1">
         <f t="array" ref="B12:CX12">MID(A12,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -37629,7 +37612,7 @@
     </row>
     <row r="13" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" t="str" cm="1">
         <f t="array" ref="B13:CX13">MID(A13,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -37938,7 +37921,7 @@
     </row>
     <row r="14" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="str" cm="1">
         <f t="array" ref="B14:CX14">MID(A14,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -38247,7 +38230,7 @@
     </row>
     <row r="15" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="str" cm="1">
         <f t="array" ref="B15:CX15">MID(A15,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -38556,7 +38539,7 @@
     </row>
     <row r="16" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" t="str" cm="1">
         <f t="array" ref="B16:CX16">MID(A16,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -38865,7 +38848,7 @@
     </row>
     <row r="17" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" t="str" cm="1">
         <f t="array" ref="B17:CX17">MID(A17,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -39174,7 +39157,7 @@
     </row>
     <row r="18" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="str" cm="1">
         <f t="array" ref="B18:CX18">MID(A18,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -39483,7 +39466,7 @@
     </row>
     <row r="19" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" t="str" cm="1">
         <f t="array" ref="B19:CX19">MID(A19,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -39792,7 +39775,7 @@
     </row>
     <row r="20" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" t="str" cm="1">
         <f t="array" ref="B20:CX20">MID(A20,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -40101,7 +40084,7 @@
     </row>
     <row r="21" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21:CX21">MID(A21,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -40410,7 +40393,7 @@
     </row>
     <row r="22" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" t="str" cm="1">
         <f t="array" ref="B22:CX22">MID(A22,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -40719,7 +40702,7 @@
     </row>
     <row r="23" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="str" cm="1">
         <f t="array" ref="B23:CX23">MID(A23,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -41028,7 +41011,7 @@
     </row>
     <row r="24" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="str" cm="1">
         <f t="array" ref="B24:CX24">MID(A24,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -41337,7 +41320,7 @@
     </row>
     <row r="25" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" t="str" cm="1">
         <f t="array" ref="B25:CX25">MID(A25,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -41646,7 +41629,7 @@
     </row>
     <row r="26" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" t="str" cm="1">
         <f t="array" ref="B26:CX26">MID(A26,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -41955,7 +41938,7 @@
     </row>
     <row r="27" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27:CX27">MID(A27,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -42264,7 +42247,7 @@
     </row>
     <row r="28" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="str" cm="1">
         <f t="array" ref="B28:CX28">MID(A28,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -42573,7 +42556,7 @@
     </row>
     <row r="29" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" t="str" cm="1">
         <f t="array" ref="B29:CX29">MID(A29,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -42882,7 +42865,7 @@
     </row>
     <row r="30" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" t="str" cm="1">
         <f t="array" ref="B30:CX30">MID(A30,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -43191,7 +43174,7 @@
     </row>
     <row r="31" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B31" t="str" cm="1">
         <f t="array" ref="B31:CX31">MID(A31,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -43500,7 +43483,7 @@
     </row>
     <row r="32" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" t="str" cm="1">
         <f t="array" ref="B32:CX32">MID(A32,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -43809,7 +43792,7 @@
     </row>
     <row r="33" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" t="str" cm="1">
         <f t="array" ref="B33:CX33">MID(A33,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -44118,7 +44101,7 @@
     </row>
     <row r="34" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" t="str" cm="1">
         <f t="array" ref="B34:CX34">MID(A34,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -44427,7 +44410,7 @@
     </row>
     <row r="35" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" t="str" cm="1">
         <f t="array" ref="B35:CX35">MID(A35,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -44736,7 +44719,7 @@
     </row>
     <row r="36" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" t="str" cm="1">
         <f t="array" ref="B36:CX36">MID(A36,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -45045,7 +45028,7 @@
     </row>
     <row r="37" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" t="str" cm="1">
         <f t="array" ref="B37:CX37">MID(A37,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -45354,7 +45337,7 @@
     </row>
     <row r="38" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" t="str" cm="1">
         <f t="array" ref="B38:CX38">MID(A38,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -45663,7 +45646,7 @@
     </row>
     <row r="39" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" t="str" cm="1">
         <f t="array" ref="B39:CX39">MID(A39,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -45972,7 +45955,7 @@
     </row>
     <row r="40" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" t="str" cm="1">
         <f t="array" ref="B40:CX40">MID(A40,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -46281,7 +46264,7 @@
     </row>
     <row r="41" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" t="str" cm="1">
         <f t="array" ref="B41:CX41">MID(A41,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -46590,7 +46573,7 @@
     </row>
     <row r="42" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B42" t="str" cm="1">
         <f t="array" ref="B42:CX42">MID(A42,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -46899,7 +46882,7 @@
     </row>
     <row r="43" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B43" t="str" cm="1">
         <f t="array" ref="B43:CX43">MID(A43,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -47208,7 +47191,7 @@
     </row>
     <row r="44" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B44" t="str" cm="1">
         <f t="array" ref="B44:CX44">MID(A44,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -47517,7 +47500,7 @@
     </row>
     <row r="45" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B45" t="str" cm="1">
         <f t="array" ref="B45:CX45">MID(A45,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -47826,7 +47809,7 @@
     </row>
     <row r="46" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B46" t="str" cm="1">
         <f t="array" ref="B46:CX46">MID(A46,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -48135,7 +48118,7 @@
     </row>
     <row r="47" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B47" t="str" cm="1">
         <f t="array" ref="B47:CX47">MID(A47,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -48444,7 +48427,7 @@
     </row>
     <row r="48" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B48" t="str" cm="1">
         <f t="array" ref="B48:CX48">MID(A48,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -48753,7 +48736,7 @@
     </row>
     <row r="49" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" t="str" cm="1">
         <f t="array" ref="B49:CX49">MID(A49,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -49062,7 +49045,7 @@
     </row>
     <row r="50" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B50" t="str" cm="1">
         <f t="array" ref="B50:CX50">MID(A50,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -49370,8 +49353,8 @@
       </c>
     </row>
     <row r="51" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>123</v>
+      <c r="A51" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="B51" t="str" cm="1">
         <f t="array" ref="B51:CX51">MID(A51,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -49680,7 +49663,7 @@
     </row>
     <row r="52" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B52" t="str" cm="1">
         <f t="array" ref="B52:CX52">MID(A52,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -49989,7 +49972,7 @@
     </row>
     <row r="53" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B53" t="str" cm="1">
         <f t="array" ref="B53:CX53">MID(A53,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -50298,7 +50281,7 @@
     </row>
     <row r="54" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B54" t="str" cm="1">
         <f t="array" ref="B54:CX54">MID(A54,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -50607,7 +50590,7 @@
     </row>
     <row r="55" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B55" t="str" cm="1">
         <f t="array" ref="B55:CX55">MID(A55,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -50916,7 +50899,7 @@
     </row>
     <row r="56" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B56" t="str" cm="1">
         <f t="array" ref="B56:CX56">MID(A56,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -51225,7 +51208,7 @@
     </row>
     <row r="57" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B57" t="str" cm="1">
         <f t="array" ref="B57:CX57">MID(A57,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -51534,7 +51517,7 @@
     </row>
     <row r="58" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B58" t="str" cm="1">
         <f t="array" ref="B58:CX58">MID(A58,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -51843,7 +51826,7 @@
     </row>
     <row r="59" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" t="str" cm="1">
         <f t="array" ref="B59:CX59">MID(A59,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -52152,7 +52135,7 @@
     </row>
     <row r="60" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B60" t="str" cm="1">
         <f t="array" ref="B60:CX60">MID(A60,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -52461,7 +52444,7 @@
     </row>
     <row r="61" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B61" t="str" cm="1">
         <f t="array" ref="B61:CX61">MID(A61,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -52770,7 +52753,7 @@
     </row>
     <row r="62" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B62" t="str" cm="1">
         <f t="array" ref="B62:CX62">MID(A62,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -53079,7 +53062,7 @@
     </row>
     <row r="63" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B63" t="str" cm="1">
         <f t="array" ref="B63:CX63">MID(A63,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -53388,7 +53371,7 @@
     </row>
     <row r="64" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B64" t="str" cm="1">
         <f t="array" ref="B64:CX64">MID(A64,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -53697,7 +53680,7 @@
     </row>
     <row r="65" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B65" t="str" cm="1">
         <f t="array" ref="B65:CX65">MID(A65,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -54006,7 +53989,7 @@
     </row>
     <row r="66" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B66" t="str" cm="1">
         <f t="array" ref="B66:CX66">MID(A66,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -54315,7 +54298,7 @@
     </row>
     <row r="67" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B67" t="str" cm="1">
         <f t="array" ref="B67:CX67">MID(A67,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -54624,7 +54607,7 @@
     </row>
     <row r="68" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B68" t="str" cm="1">
         <f t="array" ref="B68:CX68">MID(A68,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -54933,7 +54916,7 @@
     </row>
     <row r="69" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B69" t="str" cm="1">
         <f t="array" ref="B69:CX69">MID(A69,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -55242,7 +55225,7 @@
     </row>
     <row r="70" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B70" t="str" cm="1">
         <f t="array" ref="B70:CX70">MID(A70,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -55551,7 +55534,7 @@
     </row>
     <row r="71" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B71" t="str" cm="1">
         <f t="array" ref="B71:CX71">MID(A71,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -55860,7 +55843,7 @@
     </row>
     <row r="72" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B72" t="str" cm="1">
         <f t="array" ref="B72:CX72">MID(A72,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -56169,7 +56152,7 @@
     </row>
     <row r="73" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B73" t="str" cm="1">
         <f t="array" ref="B73:CX73">MID(A73,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -56478,7 +56461,7 @@
     </row>
     <row r="74" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B74" t="str" cm="1">
         <f t="array" ref="B74:CX74">MID(A74,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -56787,7 +56770,7 @@
     </row>
     <row r="75" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B75" t="str" cm="1">
         <f t="array" ref="B75:CX75">MID(A75,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -57096,7 +57079,7 @@
     </row>
     <row r="76" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B76" t="str" cm="1">
         <f t="array" ref="B76:CX76">MID(A76,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -57405,7 +57388,7 @@
     </row>
     <row r="77" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B77" t="str" cm="1">
         <f t="array" ref="B77:CX77">MID(A77,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -57714,7 +57697,7 @@
     </row>
     <row r="78" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B78" t="str" cm="1">
         <f t="array" ref="B78:CX78">MID(A78,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -58023,7 +58006,7 @@
     </row>
     <row r="79" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B79" t="str" cm="1">
         <f t="array" ref="B79:CX79">MID(A79,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -58332,7 +58315,7 @@
     </row>
     <row r="80" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B80" t="str" cm="1">
         <f t="array" ref="B80:CX80">MID(A80,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -58641,7 +58624,7 @@
     </row>
     <row r="81" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B81" t="str" cm="1">
         <f t="array" ref="B81:CX81">MID(A81,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -58950,7 +58933,7 @@
     </row>
     <row r="82" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B82" t="str" cm="1">
         <f t="array" ref="B82:CX82">MID(A82,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -59259,7 +59242,7 @@
     </row>
     <row r="83" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B83" t="str" cm="1">
         <f t="array" ref="B83:CX83">MID(A83,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -59568,7 +59551,7 @@
     </row>
     <row r="84" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B84" t="str" cm="1">
         <f t="array" ref="B84:CX84">MID(A84,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -59877,7 +59860,7 @@
     </row>
     <row r="85" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B85" t="str" cm="1">
         <f t="array" ref="B85:CX85">MID(A85,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -60186,7 +60169,7 @@
     </row>
     <row r="86" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B86" t="str" cm="1">
         <f t="array" ref="B86:CX86">MID(A86,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -60495,7 +60478,7 @@
     </row>
     <row r="87" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B87" t="str" cm="1">
         <f t="array" ref="B87:CX87">MID(A87,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -60804,7 +60787,7 @@
     </row>
     <row r="88" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B88" t="str" cm="1">
         <f t="array" ref="B88:CX88">MID(A88,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -61113,7 +61096,7 @@
     </row>
     <row r="89" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B89" t="str" cm="1">
         <f t="array" ref="B89:CX89">MID(A89,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -61422,7 +61405,7 @@
     </row>
     <row r="90" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B90" t="str" cm="1">
         <f t="array" ref="B90:CX90">MID(A90,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -61731,7 +61714,7 @@
     </row>
     <row r="91" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B91" t="str" cm="1">
         <f t="array" ref="B91:CX91">MID(A91,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -62040,7 +62023,7 @@
     </row>
     <row r="92" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B92" t="str" cm="1">
         <f t="array" ref="B92:CX92">MID(A92,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -62349,7 +62332,7 @@
     </row>
     <row r="93" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B93" t="str" cm="1">
         <f t="array" ref="B93:CX93">MID(A93,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -62658,7 +62641,7 @@
     </row>
     <row r="94" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B94" t="str" cm="1">
         <f t="array" ref="B94:CX94">MID(A94,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -62967,7 +62950,7 @@
     </row>
     <row r="95" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B95" t="str" cm="1">
         <f t="array" ref="B95:CX95">MID(A95,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -63276,7 +63259,7 @@
     </row>
     <row r="96" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B96" t="str" cm="1">
         <f t="array" ref="B96:CX96">MID(A96,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -63585,7 +63568,7 @@
     </row>
     <row r="97" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B97" t="str" cm="1">
         <f t="array" ref="B97:CX97">MID(A97,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -63894,7 +63877,7 @@
     </row>
     <row r="98" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B98" t="str" cm="1">
         <f t="array" ref="B98:CX98">MID(A98,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -64203,7 +64186,7 @@
     </row>
     <row r="99" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B99" t="str" cm="1">
         <f t="array" ref="B99:CX99">MID(A99,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -64512,7 +64495,7 @@
     </row>
     <row r="100" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B100" t="str" cm="1">
         <f t="array" ref="B100:CX100">MID(A100,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -64821,7 +64804,7 @@
     </row>
     <row r="101" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B101" t="str" cm="1">
         <f t="array" ref="B101:CX101">MID(A101,_xlfn.ANCHORARRAY(B$1),1)</f>
@@ -65129,8 +65112,8 @@
       </c>
     </row>
     <row r="102" spans="1:102" x14ac:dyDescent="0.35">
-      <c r="A102" s="5" t="s">
-        <v>124</v>
+      <c r="A102" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="B102" t="str" cm="1">
         <f t="array" ref="B102:CX102">MID(A102,_xlfn.ANCHORARRAY(B$1),1)</f>

</xml_diff>